<commit_message>
Mise en Place Css Fiche.php
</commit_message>
<xml_diff>
--- a/Documentation/Suivi_VLyon.xlsx
+++ b/Documentation/Suivi_VLyon.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1000" yWindow="-440" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="-1005" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>Mots-clé</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>maquette.pdf</t>
-  </si>
-  <si>
-    <t>Accueil/ connexion/ fiche intervention</t>
   </si>
   <si>
     <t>Liste Stations/ Detail Station/ Modif etat velo</t>
@@ -133,14 +130,32 @@
     <t>Libellé de la tache</t>
   </si>
   <si>
-    <t>Gantt</t>
+    <t>Accueil/ connexion/ fiche intervention/ Demande d'intervnetion</t>
+  </si>
+  <si>
+    <t>Gestion des Stations - Etat velo</t>
+  </si>
+  <si>
+    <t>Gestion des commandes</t>
+  </si>
+  <si>
+    <t>Gestion des Demandes d'interventions</t>
+  </si>
+  <si>
+    <t>Gestion des Bons d'interventions</t>
+  </si>
+  <si>
+    <t>Mise en place de contrôles de saisies</t>
+  </si>
+  <si>
+    <t>Mise en place d'une interface mobile - Css</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +223,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +242,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -308,7 +335,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,8 +347,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -364,6 +392,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,11 +404,23 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="11" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -389,9 +432,15 @@
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="11" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -680,52 +729,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.1640625" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="14">
-        <v>41564</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -740,12 +767,14 @@
       <c r="K2" s="14">
         <v>41564</v>
       </c>
-      <c r="L2" s="15"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="L2" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -757,15 +786,15 @@
       <c r="J3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="16">
-        <v>41585</v>
+      <c r="K3" s="14">
+        <v>41564</v>
       </c>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -782,10 +811,10 @@
       </c>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -802,432 +831,662 @@
       </c>
       <c r="L5" s="15"/>
     </row>
-    <row r="7" spans="1:12" ht="15">
-      <c r="A7" s="9" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="16">
+        <v>41585</v>
+      </c>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="25"/>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J13" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L13" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15">
-      <c r="A8" s="20" t="s">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" ht="15">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="23"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="15">
-      <c r="A11" s="2"/>
-      <c r="B11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="15">
-      <c r="A12" s="2"/>
-      <c r="B12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="15">
-      <c r="A13" s="2"/>
-      <c r="B13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="15">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="4"/>
+      <c r="J15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="14">
+        <v>41564</v>
+      </c>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="1:12" ht="15">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="4"/>
+      <c r="J16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="14">
+        <v>41564</v>
+      </c>
       <c r="L16" s="11"/>
     </row>
-    <row r="17" spans="1:12" ht="15">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
+      <c r="B17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="4"/>
+      <c r="J17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="16">
+        <v>41585</v>
+      </c>
       <c r="L17" s="11"/>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="4"/>
+      <c r="J18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="16">
+        <v>41585</v>
+      </c>
       <c r="L18" s="11"/>
     </row>
-    <row r="19" spans="1:12" ht="15">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="4"/>
+      <c r="J19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="16">
+        <v>41585</v>
+      </c>
       <c r="L19" s="11"/>
     </row>
-    <row r="20" spans="1:12" ht="15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="2"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="4"/>
+      <c r="J20" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="28">
+        <v>41585</v>
+      </c>
       <c r="L20" s="11"/>
     </row>
-    <row r="21" spans="1:12" ht="15">
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="27" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="3"/>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="J21" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="K21" s="28">
+        <v>41585</v>
+      </c>
       <c r="L21" s="11"/>
     </row>
-    <row r="22" spans="1:12" ht="15">
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="27" t="s">
+        <v>32</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="F22" s="29"/>
+      <c r="H22" s="29"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="10"/>
+      <c r="J22" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="28">
+        <v>41585</v>
+      </c>
       <c r="L22" s="11"/>
     </row>
-    <row r="23" spans="1:12" ht="15">
-      <c r="A23" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="22"/>
-    </row>
-    <row r="24" spans="1:12" ht="15">
-      <c r="A24" s="8"/>
-      <c r="B24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>23</v>
-      </c>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="28">
+        <v>41599</v>
+      </c>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="F24" s="29"/>
+      <c r="H24" s="30"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="28">
+        <v>41606</v>
+      </c>
       <c r="L24" s="11"/>
     </row>
-    <row r="25" spans="1:12" ht="15">
-      <c r="A25" s="12"/>
-      <c r="B25" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>24</v>
-      </c>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="2"/>
+      <c r="F25" s="29"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="28">
+        <v>41606</v>
+      </c>
       <c r="L25" s="11"/>
     </row>
-    <row r="26" spans="1:12" ht="15">
-      <c r="A26" s="12"/>
-      <c r="B26" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>25</v>
-      </c>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="2"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="28"/>
       <c r="L26" s="11"/>
     </row>
-    <row r="27" spans="1:12" ht="15">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="2"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="28"/>
       <c r="L27" s="11"/>
     </row>
-    <row r="28" spans="1:12" ht="15">
-      <c r="A28" s="12"/>
-      <c r="B28" s="23" t="s">
-        <v>30</v>
-      </c>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="4"/>
       <c r="L28" s="11"/>
     </row>
-    <row r="29" spans="1:12" ht="15">
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="7"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="4"/>
       <c r="L29" s="11"/>
     </row>
-    <row r="30" spans="1:12" ht="15">
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="4"/>
       <c r="L30" s="11"/>
     </row>
-    <row r="31" spans="1:12" ht="15">
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="4"/>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:12" ht="15">
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="4"/>
       <c r="L32" s="11"/>
     </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="11"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="23"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="11"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="11"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="11"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="11"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>